<commit_message>
Add 3rd year and 2nd year subjects
</commit_message>
<xml_diff>
--- a/cs-gradings.xlsx
+++ b/cs-gradings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raminduwalgama/Desktop/Projects/uni_ranker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raminduwalgama/Documents/Projects/uni_ranker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F6A777-3C92-834F-8BF8-66872CE57F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78FD394-34E3-DA46-8C58-6C3013894AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="-1460" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18000" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subject_info" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>SCS 1201</t>
   </si>
@@ -207,13 +207,145 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Machine Learning and Neural Computing</t>
+  </si>
+  <si>
+    <t>SCS 3201</t>
+  </si>
+  <si>
+    <t>SCS 3202</t>
+  </si>
+  <si>
+    <t>SCS 3203</t>
+  </si>
+  <si>
+    <t>SCS 3204</t>
+  </si>
+  <si>
+    <t>SCS 3205</t>
+  </si>
+  <si>
+    <t>SCS 3206</t>
+  </si>
+  <si>
+    <t>SCS 3207</t>
+  </si>
+  <si>
+    <t>Advanced Computer Architecture</t>
+  </si>
+  <si>
+    <t>Middleware Architecture</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Computer Graphics I</t>
+  </si>
+  <si>
+    <t>Graph Theory</t>
+  </si>
+  <si>
+    <t>Software Quality Assurance</t>
+  </si>
+  <si>
+    <t>SCS 3208</t>
+  </si>
+  <si>
+    <t>SCS 3209</t>
+  </si>
+  <si>
+    <t>SCS 3210</t>
+  </si>
+  <si>
+    <t>Software Project Management</t>
+  </si>
+  <si>
+    <t>Human Computer Interaction</t>
+  </si>
+  <si>
+    <t>Systems and Network Administration</t>
+  </si>
+  <si>
+    <t>SCS 3211</t>
+  </si>
+  <si>
+    <t>SCS 3212</t>
+  </si>
+  <si>
+    <t>SCS 3213</t>
+  </si>
+  <si>
+    <t>SCS 3214</t>
+  </si>
+  <si>
+    <t>SCS 3215</t>
+  </si>
+  <si>
+    <t>SCS 3216</t>
+  </si>
+  <si>
+    <t>Compiler Theory</t>
+  </si>
+  <si>
+    <t>Mobile Application Development</t>
+  </si>
+  <si>
+    <t>Game Development</t>
+  </si>
+  <si>
+    <t>Group Project II</t>
+  </si>
+  <si>
+    <t>Professional Practice</t>
+  </si>
+  <si>
+    <t>Research Methods</t>
+  </si>
+  <si>
+    <t>SCS 2209</t>
+  </si>
+  <si>
+    <t>Database II</t>
+  </si>
+  <si>
+    <t>SCS 2210</t>
+  </si>
+  <si>
+    <t>Discrete Mathematics II</t>
+  </si>
+  <si>
+    <t>Laboratory II</t>
+  </si>
+  <si>
+    <t>SCS 2211</t>
+  </si>
+  <si>
+    <t>SCS 2212</t>
+  </si>
+  <si>
+    <t>SCS 2213</t>
+  </si>
+  <si>
+    <t>Electronics and Physical Computing</t>
+  </si>
+  <si>
+    <t>Automata Theory</t>
+  </si>
+  <si>
+    <t>SCS 2214</t>
+  </si>
+  <si>
+    <t>Information System Security</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -224,6 +356,19 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -365,7 +510,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -410,6 +555,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1571,16 +1725,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.33203125" style="1"/>
@@ -1837,6 +1991,248 @@
       </c>
       <c r="C23" s="8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1855,7 +2251,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>